<commit_message>
Adjusted Test Cases and Exported Postman collection
</commit_message>
<xml_diff>
--- a/Test Task.xlsx
+++ b/Test Task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enthropy\Desktop\testask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300FCF57-4FFC-4987-97E0-AC62F90C2AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D01AFE-7894-4D35-BA7C-AE2912A8B343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,10 +283,6 @@
   <si>
     <t>HTTP Method: GET
 URL: https://restful-booker.herokuapp.com/ping?value=test</t>
-  </si>
-  <si>
-    <t>HTTP Method: GET
-URL: https://restful-booker.herokuapp.com/ping</t>
   </si>
   <si>
     <t>HTTP Method: POST
@@ -852,6 +848,10 @@
     <t>1. Запрос успешно отправлен;
 2. Статус-код 400 Bad Request;
 3. В теле ответа возвращается "Bad Request".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTTP Method: GET
+URL: https://restful-booker.herokuapp.com/ping </t>
   </si>
 </sst>
 </file>
@@ -1488,7 +1488,7 @@
     </row>
     <row r="3" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="5" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
@@ -1539,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>11</v>
@@ -1548,7 +1548,7 @@
         <v>18</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>19</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="6" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>7</v>
@@ -1566,7 +1566,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>11</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="8" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
@@ -1609,7 +1609,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>14</v>
@@ -1618,18 +1618,18 @@
         <v>18</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
@@ -1638,7 +1638,7 @@
         <v>23</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>24</v>
@@ -1647,7 +1647,7 @@
         <v>18</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>15</v>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="10" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>17</v>
@@ -1665,7 +1665,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>25</v>
@@ -1674,7 +1674,7 @@
         <v>18</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>15</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="11" spans="1:14" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
@@ -1692,7 +1692,7 @@
         <v>26</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>32</v>
@@ -1701,7 +1701,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>15</v>
@@ -1807,70 +1807,70 @@
     </row>
     <row r="5" spans="1:10" ht="360.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:10" ht="363.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>42</v>
@@ -1879,56 +1879,56 @@
         <v>28</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="I8" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>43</v>
@@ -1937,7 +1937,7 @@
         <v>28</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>47</v>
@@ -1946,16 +1946,16 @@
     </row>
     <row r="10" spans="1:10" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>44</v>
@@ -1964,7 +1964,7 @@
         <v>45</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>48</v>
@@ -1973,16 +1973,16 @@
     </row>
     <row r="11" spans="1:10" ht="268.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>43</v>
@@ -1991,13 +1991,13 @@
         <v>46</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2016,227 +2016,227 @@
     </row>
     <row r="13" spans="1:10" ht="258" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="290.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="249" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>41</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="289.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18" s="7" t="s">
+      <c r="F18" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="G18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="I18" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>91</v>
-      </c>
       <c r="G19" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:9" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="F20" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I20" s="17"/>
     </row>
@@ -2284,7 +2284,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,16 +2367,16 @@
     </row>
     <row r="5" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>52</v>
+        <v>153</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>27</v>
@@ -2385,18 +2385,18 @@
         <v>28</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>36</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>17</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="8" spans="1:9" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>17</v>
@@ -2445,7 +2445,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>34</v>
@@ -2460,7 +2460,7 @@
         <v>38</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>